<commit_message>
Cleaned up the text in the article.
</commit_message>
<xml_diff>
--- a/reactionDataTest2.xlsx
+++ b/reactionDataTest2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Jupyter/pyIonicEquilibrium/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1E3035-47E2-1B4A-93B0-F35682EDD895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC56D47D-B1D4-334C-A647-93FF69D828D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1860" windowWidth="23200" windowHeight="15060" xr2:uid="{48EA54D9-7A74-9C47-A53B-B305778769D4}"/>
+    <workbookView xWindow="5600" yWindow="1360" windowWidth="23200" windowHeight="15060" activeTab="1" xr2:uid="{48EA54D9-7A74-9C47-A53B-B305778769D4}"/>
   </bookViews>
   <sheets>
     <sheet name="speciesDataShort" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>species</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>HS-</t>
-  </si>
-  <si>
-    <t>CO2</t>
   </si>
   <si>
     <t>HCO3-</t>
@@ -509,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA93B94-611B-544B-8CF7-0E3D27E2E904}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -520,44 +517,41 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3.0400000000000002E-3</v>
+      </c>
+      <c r="C2" s="1"/>
       <c r="D2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>3.0400000000000002E-3</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
       <c r="D3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -568,7 +562,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1">
         <v>1.02E-4</v>
@@ -580,7 +574,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -591,7 +585,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -602,10 +596,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -613,7 +610,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -624,7 +621,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <f>1000/18.015</f>
@@ -643,79 +640,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE1B8378-0DFC-AD44-90C6-383F5B4F4D5A}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="29.83203125" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" t="s">
         <v>8</v>
-      </c>
-      <c r="M1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3">
         <f>0.0000000089</f>
         <v>8.9000000000000003E-9</v>
       </c>
       <c r="E2" s="2">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F2" s="2">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="2">
         <v>0</v>
@@ -727,10 +723,10 @@
         <v>0</v>
       </c>
       <c r="K2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" s="2">
         <v>0</v>
@@ -738,38 +734,39 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="3">
-        <v>4.4999999999999998E-7</v>
+        <f>0.0000000000000000001</f>
+        <v>9.9999999999999998E-20</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
       </c>
       <c r="F3" s="2">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="2">
         <v>0</v>
       </c>
       <c r="K3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" s="2">
         <v>0</v>
@@ -780,11 +777,11 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="3">
-        <v>4.6999999999999999E-11</v>
+        <v>4.4999999999999998E-7</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -796,19 +793,19 @@
         <v>0</v>
       </c>
       <c r="H4" s="2">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I4" s="2">
         <v>1</v>
       </c>
       <c r="J4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="2">
         <v>0</v>
@@ -816,82 +813,81 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="3">
+        <v>4.6999999999999999E-11</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>-1</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="3">
         <f>1/100000000000000</f>
         <v>1E-14</v>
       </c>
-      <c r="E5" s="2">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1</v>
-      </c>
-      <c r="L5" s="2">
-        <v>0</v>
-      </c>
-      <c r="M5" s="2">
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2">
         <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="3">
-        <f>0.0000000000000000001</f>
-        <v>9.9999999999999998E-20</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>-1</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0</v>
-      </c>
-      <c r="K6" s="2">
-        <v>1</v>
-      </c>
-      <c r="L6" s="2">
-        <v>1</v>
-      </c>
-      <c r="M6" s="2">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>